<commit_message>
Commiting Upto date Project contents
</commit_message>
<xml_diff>
--- a/DataLibrary.xlsx
+++ b/DataLibrary.xlsx
@@ -26,13 +26,13 @@
     <sheet name="TUITION REIMBURSEMENT SUITE" r:id="rId35" sheetId="207"/>
     <sheet name="PAYROLL REQUEST SUITE" r:id="rId41" sheetId="208"/>
     <sheet name="SECURITY SUITE" r:id="rId43" sheetId="220"/>
-    <sheet name="KNOWLEDGE BASE SUITE" r:id="rId29" sheetId="236"/>
     <sheet name="CASE MANAGEMENT SUITE" r:id="rId30" sheetId="237"/>
     <sheet name="SECURITY SUITE - 1" r:id="rId36" sheetId="238"/>
     <sheet name="SECURITY SUITE - 3" r:id="rId38" sheetId="240"/>
     <sheet name="SECURITY SUITE - 2" r:id="rId37" sheetId="241"/>
     <sheet name="Default suite" r:id="rId39" sheetId="242"/>
     <sheet name="GENERAL INQUIRY SUITE" r:id="rId32" sheetId="243"/>
+    <sheet name="KNOWLEDGE BASE SUITE" r:id="rId29" sheetId="244"/>
   </sheets>
   <calcPr calcId="125725"/>
   <smartTagPr show="none"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="375">
   <si>
     <t>Identifier Variables</t>
   </si>
@@ -2045,35 +2045,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet236.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet237.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B1"/>
@@ -2200,6 +2171,27 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet244.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>

</xml_diff>